<commit_message>
Add per-camp provider breakdown to budget summary and fix camp fee formulas
Budget Summary spreadsheet: Camp Fees now use SUM formulas referencing the
Weekly Schedule tab instead of hardcoded values, and a new "Cost by Camp
Provider" section uses SUMIF formulas to break down costs by provider per child.
Budget-optimization skill: added per-camp breakdown to the markdown template,
corrected example numbers, and replaced external xlsx skill dependency with a
reference to the sample Excel template.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/kids-camp-planner/examples/sample-budget.xlsx
+++ b/kids-camp-planner/examples/sample-budget.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t xml:space="preserve">Summer 2025 Camp Budget</t>
   </si>
@@ -114,6 +114,24 @@
     <t xml:space="preserve">Total Savings</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost by Camp Provider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YMCA Cedar Glen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City of Toronto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Camp TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Camp Fees</t>
+  </si>
+  <si>
     <t xml:space="preserve">Summer 2025 Weekly Schedule</t>
   </si>
   <si>
@@ -141,9 +159,6 @@
     <t xml:space="preserve">Jun 30 - Jul 4</t>
   </si>
   <si>
-    <t xml:space="preserve">YMCA Cedar Glen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jul 7 - Jul 11</t>
   </si>
   <si>
@@ -153,9 +168,6 @@
     <t xml:space="preserve">Jul 21 - Jul 25</t>
   </si>
   <si>
-    <t xml:space="preserve">City of Toronto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jul 28 - Aug 1</t>
   </si>
   <si>
@@ -165,9 +177,6 @@
     <t xml:space="preserve">Aug 11 - Aug 15</t>
   </si>
   <si>
-    <t xml:space="preserve">Science Camp TO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aug 18 - Aug 22</t>
   </si>
   <si>
@@ -175,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">Camp Provider Comparison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provider</t>
   </si>
   <si>
     <t xml:space="preserve">Weekly Cost</t>
@@ -244,7 +250,7 @@
     <numFmt numFmtId="166" formatCode="\$#,##0;&quot;($&quot;#,##0\);\-"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,7 +303,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -305,6 +311,13 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -321,6 +334,14 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF2C3E50"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -411,16 +432,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,115 +453,159 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,7 +617,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -805,7 +874,7 @@
     <tabColor rgb="FF2C3E50"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -813,309 +882,398 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="18"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>2400</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>2400</v>
-      </c>
-      <c r="D5" s="6" t="n">
+      <c r="B5" s="6" t="n">
+        <f aca="false">SUM('Weekly Schedule'!D4:D11)</f>
+        <v>2350</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <f aca="false">SUM('Weekly Schedule'!F4:F11)</f>
+        <v>2200</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <f aca="false">B5+C5</f>
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="10" t="n">
         <f aca="false">B6+C6</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="11" t="n">
         <v>280</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="11" t="n">
         <v>280</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <f aca="false">B7+C7</f>
         <v>560</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="C8" s="8" t="n">
+      <c r="C8" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="10" t="n">
         <f aca="false">B8+C8</f>
         <v>100</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="13" t="n">
         <f aca="false">SUM(B5:B8)</f>
-        <v>3530</v>
-      </c>
-      <c r="C9" s="11" t="n">
+        <v>3480</v>
+      </c>
+      <c r="C9" s="13" t="n">
         <f aca="false">SUM(C5:C8)</f>
-        <v>3530</v>
-      </c>
-      <c r="D9" s="11" t="n">
+        <v>3330</v>
+      </c>
+      <c r="D9" s="13" t="n">
         <f aca="false">SUM(D5:D8)</f>
-        <v>7060</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+        <v>6810</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="14" t="n">
+      <c r="B13" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="14" t="n">
+      <c r="C13" s="16" t="n">
         <v>240</v>
       </c>
-      <c r="D13" s="15" t="n">
+      <c r="D13" s="17" t="n">
         <f aca="false">B13+C13</f>
         <v>240</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="16" t="n">
+      <c r="B14" s="18" t="n">
         <v>200</v>
       </c>
-      <c r="C14" s="16" t="n">
+      <c r="C14" s="18" t="n">
         <v>200</v>
       </c>
-      <c r="D14" s="17" t="n">
+      <c r="D14" s="19" t="n">
         <f aca="false">B14+C14</f>
         <v>400</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="19" t="n">
+      <c r="B15" s="21" t="n">
         <f aca="false">SUM(B13:B14)</f>
         <v>200</v>
       </c>
-      <c r="C15" s="19" t="n">
+      <c r="C15" s="21" t="n">
         <f aca="false">SUM(C13:C14)</f>
         <v>440</v>
       </c>
-      <c r="D15" s="19" t="n">
+      <c r="D15" s="21" t="n">
         <f aca="false">SUM(D13:D14)</f>
         <v>640</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="21" t="n">
+      <c r="B17" s="23" t="n">
         <f aca="false">B9-B15</f>
-        <v>3330</v>
-      </c>
-      <c r="C17" s="21" t="n">
+        <v>3280</v>
+      </c>
+      <c r="C17" s="23" t="n">
         <f aca="false">C9-C15</f>
-        <v>3090</v>
-      </c>
-      <c r="D17" s="21" t="n">
+        <v>2890</v>
+      </c>
+      <c r="D17" s="23" t="n">
         <f aca="false">D9-D15</f>
-        <v>6420</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+        <v>6170</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="23" t="n">
+      <c r="B20" s="25" t="n">
         <v>7000</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="24" t="n">
+      <c r="B21" s="26" t="n">
         <f aca="false">D17</f>
-        <v>6420</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
+        <v>6170</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="26" t="n">
+      <c r="B22" s="28" t="n">
         <f aca="false">B20-B21</f>
-        <v>580</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="27" t="str">
+      <c r="B23" s="29" t="str">
         <f aca="false">IF(B22&gt;=0,"UNDER BUDGET","OVER BUDGET")</f>
         <v>UNDER BUDGET</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="24" t="n">
+      <c r="B27" s="26" t="n">
         <f aca="false">B17</f>
-        <v>3330</v>
-      </c>
-      <c r="C27" s="28" t="n">
+        <v>3280</v>
+      </c>
+      <c r="C27" s="30" t="n">
         <v>0.25</v>
       </c>
-      <c r="D27" s="24" t="n">
+      <c r="D27" s="26" t="n">
         <f aca="false">B27*C27</f>
-        <v>832.5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="29" t="n">
+      <c r="B28" s="31" t="n">
         <f aca="false">C17</f>
-        <v>3090</v>
-      </c>
-      <c r="C28" s="30" t="n">
+        <v>2890</v>
+      </c>
+      <c r="C28" s="32" t="n">
         <v>0.25</v>
       </c>
-      <c r="D28" s="29" t="n">
+      <c r="D28" s="31" t="n">
         <f aca="false">B28*C28</f>
-        <v>772.5</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+        <v>722.5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="11" t="n">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="13" t="n">
         <f aca="false">SUM(D27:D28)</f>
-        <v>1605</v>
+        <v>1542.5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="37" t="n">
+        <f aca="false">SUMIF('Weekly Schedule'!C$4:C$11,A33,'Weekly Schedule'!D$4:D$11)</f>
+        <v>1800</v>
+      </c>
+      <c r="C33" s="37" t="n">
+        <f aca="false">SUMIF('Weekly Schedule'!E$4:E$11,A33,'Weekly Schedule'!F$4:F$11)</f>
+        <v>1800</v>
+      </c>
+      <c r="D33" s="38" t="n">
+        <f aca="false">B33+C33</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="40" t="n">
+        <f aca="false">SUMIF('Weekly Schedule'!C$4:C$11,A34,'Weekly Schedule'!D$4:D$11)</f>
+        <v>200</v>
+      </c>
+      <c r="C34" s="40" t="n">
+        <f aca="false">SUMIF('Weekly Schedule'!E$4:E$11,A34,'Weekly Schedule'!F$4:F$11)</f>
+        <v>400</v>
+      </c>
+      <c r="D34" s="41" t="n">
+        <f aca="false">B34+C34</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="37" t="n">
+        <f aca="false">SUMIF('Weekly Schedule'!C$4:C$11,A35,'Weekly Schedule'!D$4:D$11)</f>
+        <v>350</v>
+      </c>
+      <c r="C35" s="37" t="n">
+        <f aca="false">SUMIF('Weekly Schedule'!E$4:E$11,A35,'Weekly Schedule'!F$4:F$11)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="38" t="n">
+        <f aca="false">B35+C35</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="43" t="n">
+        <f aca="false">SUM(B33:B35)</f>
+        <v>2350</v>
+      </c>
+      <c r="C36" s="43" t="n">
+        <f aca="false">SUM(C33:C35)</f>
+        <v>2200</v>
+      </c>
+      <c r="D36" s="43" t="n">
+        <f aca="false">SUM(D33:D35)</f>
+        <v>4550</v>
       </c>
     </row>
   </sheetData>
@@ -1149,257 +1307,257 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="5" t="n">
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="7" t="n">
         <f aca="false">D4+F4</f>
         <v>600</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="n">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="8" t="n">
+      <c r="B5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="8" t="n">
+      <c r="E5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <f aca="false">D5+F5</f>
         <v>600</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="n">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="44" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="5" t="n">
+      <c r="B6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="5" t="n">
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <f aca="false">D6+F6</f>
         <v>600</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="n">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="8" t="n">
+      <c r="B7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="8" t="n">
+      <c r="E7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="10" t="n">
         <f aca="false">D7+F7</f>
         <v>400</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="n">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="44" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="5" t="n">
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="5" t="n">
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <f aca="false">D8+F8</f>
         <v>600</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="n">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="8" t="n">
+      <c r="B9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="8" t="n">
+      <c r="E9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="10" t="n">
         <f aca="false">D9+F9</f>
         <v>600</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="n">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="44" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="5" t="n">
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="11" t="n">
         <v>350</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="5" t="n">
+      <c r="E10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="11" t="n">
         <v>200</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="7" t="n">
         <f aca="false">D10+F10</f>
         <v>550</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33" t="n">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="45" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="8" t="n">
+      <c r="B11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="8" t="n">
+      <c r="E11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="10" t="n">
         <f aca="false">D11+F11</f>
         <v>600</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="11" t="n">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="13" t="n">
         <f aca="false">SUM(D4:D11)</f>
         <v>2350</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="11" t="n">
+      <c r="E12" s="33"/>
+      <c r="F12" s="13" t="n">
         <f aca="false">SUM(F4:F11)</f>
         <v>2200</v>
       </c>
-      <c r="G12" s="21" t="n">
+      <c r="G12" s="23" t="n">
         <f aca="false">SUM(G4:G11)</f>
         <v>4550</v>
       </c>
@@ -1432,222 +1590,222 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="38"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>300</v>
+      </c>
+      <c r="C4" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="C4" s="5" t="n">
+      <c r="D4" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="D4" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="7" t="n">
         <f aca="false">SUM(B4:E4)</f>
         <v>435</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="8" t="n">
+      <c r="G4" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="E5" s="18" t="n">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="10" t="n">
         <f aca="false">SUM(B5:E5)</f>
         <v>310</v>
       </c>
-      <c r="G5" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+      <c r="G5" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="H5" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="11" t="n">
         <v>350</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="7" t="n">
         <f aca="false">SUM(B6:E6)</f>
         <v>450</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="G6" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="str">
+      <c r="D9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27" t="str">
         <f aca="false">A4</f>
         <v>YMCA Cedar Glen</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="26" t="n">
         <f aca="false">B4*8</f>
         <v>2400</v>
       </c>
-      <c r="C10" s="24" t="n">
+      <c r="C10" s="26" t="n">
         <f aca="false">(B4+C4+D4)*8</f>
         <v>3200</v>
       </c>
-      <c r="D10" s="24" t="n">
+      <c r="D10" s="26" t="n">
         <f aca="false">F4*8</f>
         <v>3480</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="7" t="n">
         <f aca="false">D10</f>
         <v>3480</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="str">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="46" t="str">
         <f aca="false">A5</f>
         <v>City of Toronto</v>
       </c>
-      <c r="B11" s="29" t="n">
+      <c r="B11" s="31" t="n">
         <f aca="false">B5*8</f>
         <v>1600</v>
       </c>
-      <c r="C11" s="29" t="n">
+      <c r="C11" s="31" t="n">
         <f aca="false">(B5+C5+D5)*8</f>
         <v>2240</v>
       </c>
-      <c r="D11" s="29" t="n">
+      <c r="D11" s="31" t="n">
         <f aca="false">F5*8</f>
         <v>2480</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="10" t="n">
         <f aca="false">D11</f>
         <v>2480</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="str">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="27" t="str">
         <f aca="false">A6</f>
         <v>Science Camp Toronto</v>
       </c>
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="26" t="n">
         <f aca="false">B6*8</f>
         <v>2800</v>
       </c>
-      <c r="C12" s="24" t="n">
+      <c r="C12" s="26" t="n">
         <f aca="false">(B6+C6+D6)*8</f>
         <v>3600</v>
       </c>
-      <c r="D12" s="24" t="n">
+      <c r="D12" s="26" t="n">
         <f aca="false">F6*8</f>
         <v>3600</v>
       </c>
-      <c r="E12" s="6" t="n">
+      <c r="E12" s="7" t="n">
         <f aca="false">D12</f>
         <v>3600</v>
       </c>

</xml_diff>